<commit_message>
Add multiple files and blank attributes to test
</commit_message>
<xml_diff>
--- a/test_data/single_with_file.xlsx
+++ b/test_data/single_with_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -55,9 +55,21 @@
     <t xml:space="preserve">File: File that doesn’t exist</t>
   </si>
   <si>
+    <t xml:space="preserve">File:that exists with path:P1/D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file:P1/D1</t>
+  </si>
+  <si>
     <t xml:space="preserve">G181030g</t>
   </si>
   <si>
+    <t xml:space="preserve">n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blank</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ti-6Al-4V</t>
   </si>
   <si>
@@ -65,6 +77,12 @@
   </si>
   <si>
     <t xml:space="preserve">P1/does-not-exist.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hello2.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hello3.txt</t>
   </si>
 </sst>
 </file>
@@ -171,7 +189,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -223,6 +241,12 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="ALT1" s="0"/>
       <c r="ALU1" s="0"/>
       <c r="ALV1" s="0"/>
@@ -243,16 +267,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1.6</v>
@@ -262,13 +286,19 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>140.999779122757</v>
+        <v>142.41093380861</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -283,7 +313,9 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J1" r:id="rId1" display="FILE:File"/>
+    <hyperlink ref="J1" r:id="rId1" display="FILE:File that exists"/>
+    <hyperlink ref="L1" r:id="rId2" display="File:that"/>
+    <hyperlink ref="M1" r:id="rId3" display="file:P1/D1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>